<commit_message>
updated case study input files for Alameda Island. max time step limited for more efficient testing
</commit_message>
<xml_diff>
--- a/Example 5_business/water_distribution_network/rewet_results/SCN_.xlsx
+++ b/Example 5_business/water_distribution_network/rewet_results/SCN_.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\OneDrive - Stanford\Research\02 Work\05 Commercial downtime\Pyrecodes\pyrecodes-main\Example 5_business\water_distribution_network\rewet_results</t>
+          <t>/Users/nikola/pyrecodes_business/Example 5_business/water_distribution_network/rewet_results</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\OneDrive - Stanford\Research\02 Work\05 Commercial downtime\Pyrecodes\pyrecodes-main\Example 5_business\water_distribution_network\rewet_temp</t>
+          <t>/Users/nikola/pyrecodes_business/Example 5_business/water_distribution_network/rewet_temp</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\OneDrive - Stanford\Research\02 Work\05 Commercial downtime\Pyrecodes\pyrecodes-main\Example 5_business\water_distribution_network\waterNetwork.inp</t>
+          <t>/Users/nikola/pyrecodes_business/Example 5_business/water_distribution_network/waterNetwork.inp</t>
         </is>
       </c>
     </row>
@@ -628,7 +628,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\OneDrive - Stanford\Research\02 Work\05 Commercial downtime\Pyrecodes\pyrecodes-main\Example 5_business\water_distribution_network\rewet_temp\list.xlsx</t>
+          <t>/Users/nikola/pyrecodes_business/Example 5_business/water_distribution_network/rewet_temp/list.xlsx</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\OneDrive - Stanford\Research\02 Work\05 Commercial downtime\Pyrecodes\pyrecodes-main\Example 5_business\water_distribution_network\rewet_temp</t>
+          <t>/Users/nikola/pyrecodes_business/Example 5_business/water_distribution_network/rewet_temp</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>C:\Users\zhut\anaconda3\envs\pyrecodes_env\Lib\site-packages\rewet\examples\Net3\config.txt</t>
+          <t>/Users/nikola/pyrecodes_business/env_pyrecodes/lib/python3.9/site-packages/rewet/examples/Net3/config.txt</t>
         </is>
       </c>
     </row>

</xml_diff>